<commit_message>
- presentation - evaluation
</commit_message>
<xml_diff>
--- a/examples/Kopie von Analyse_AutoNukleolierkennung.xlsx
+++ b/examples/Kopie von Analyse_AutoNukleolierkennung.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="32">
   <si>
     <t>Auswertung: Automatische Zielerkennung</t>
   </si>
@@ -104,13 +104,19 @@
   </si>
   <si>
     <t>Bestrahlungzeit</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>Mit NuFi</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -122,6 +128,13 @@
       <b/>
       <sz val="20"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -265,7 +278,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -295,9 +308,15 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -604,29 +623,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:Q22"/>
+  <dimension ref="A2:R41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O27" sqref="O27"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="M28" sqref="M28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="14.85546875" customWidth="1"/>
     <col min="4" max="4" width="13.140625" customWidth="1"/>
-    <col min="5" max="5" width="24" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14" customWidth="1"/>
+    <col min="5" max="6" width="14" customWidth="1"/>
     <col min="7" max="7" width="15.42578125" customWidth="1"/>
     <col min="8" max="8" width="15.7109375" customWidth="1"/>
     <col min="9" max="9" width="14.5703125" customWidth="1"/>
     <col min="10" max="10" width="25.7109375" customWidth="1"/>
-    <col min="12" max="12" width="24" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.7109375" customWidth="1"/>
     <col min="16" max="16" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="14.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:17" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:18" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -634,20 +650,20 @@
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
       <c r="B4" s="3"/>
-      <c r="C4" s="29" t="s">
+      <c r="C4" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="29"/>
-      <c r="E4" s="29"/>
+      <c r="D4" s="30"/>
+      <c r="E4" s="30"/>
       <c r="F4" s="16"/>
-      <c r="G4" s="29" t="s">
+      <c r="G4" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="H4" s="29"/>
-      <c r="I4" s="29"/>
+      <c r="H4" s="30"/>
+      <c r="I4" s="30"/>
       <c r="J4" s="4" t="s">
         <v>8</v>
       </c>
@@ -659,7 +675,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
         <v>1</v>
       </c>
@@ -701,7 +717,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="6">
         <v>3</v>
       </c>
@@ -740,14 +756,17 @@
         <f>(C6-D6)/J6</f>
         <v>0.8214285714285714</v>
       </c>
-      <c r="P6" s="27">
+      <c r="P6" s="28">
         <v>0.60972222222222217</v>
       </c>
-      <c r="Q6" s="28">
+      <c r="Q6" s="29">
         <v>0.61226851851851849</v>
       </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="6">
         <v>3</v>
       </c>
@@ -786,14 +805,17 @@
         <f t="shared" ref="M7:M9" si="0">(C7-D7)/J7</f>
         <v>0.88888888888888884</v>
       </c>
-      <c r="P7" s="27">
+      <c r="P7" s="28">
         <v>0.61458333333333337</v>
       </c>
-      <c r="Q7" s="28">
+      <c r="Q7" s="29">
         <v>0.61684027777777783</v>
       </c>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="6">
         <v>3</v>
       </c>
@@ -832,14 +854,17 @@
         <f t="shared" si="0"/>
         <v>0.93939393939393945</v>
       </c>
-      <c r="P8" s="27">
+      <c r="P8" s="28">
         <v>0.61805555555555558</v>
       </c>
-      <c r="Q8" s="28">
+      <c r="Q8" s="29">
         <v>0.61962962962962964</v>
       </c>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" s="10">
         <v>3</v>
       </c>
@@ -880,19 +905,22 @@
         <f t="shared" si="0"/>
         <v>0.75</v>
       </c>
-      <c r="P9" s="27">
+      <c r="P9" s="28">
         <v>0.62013888888888891</v>
       </c>
-      <c r="Q9" s="28">
+      <c r="Q9" s="29">
         <v>0.62229166666666669</v>
       </c>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R9">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" s="18" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" s="20">
         <v>2</v>
       </c>
@@ -931,14 +959,17 @@
         <f>(C11-D11)/J11</f>
         <v>1</v>
       </c>
-      <c r="P11" s="27">
+      <c r="P11" s="28">
         <v>0.63402777777777775</v>
       </c>
-      <c r="Q11" s="28">
+      <c r="Q11" s="29">
         <v>0.63670138888888894</v>
       </c>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" s="6">
         <v>2</v>
       </c>
@@ -977,14 +1008,17 @@
         <f t="shared" ref="M12:M19" si="1">(C12-D12)/J12</f>
         <v>1</v>
       </c>
-      <c r="P12" s="27">
+      <c r="P12" s="28">
         <v>0.6381944444444444</v>
       </c>
-      <c r="Q12" s="28">
+      <c r="Q12" s="29">
         <v>0.64165509259259257</v>
       </c>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R12">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" s="6">
         <v>2</v>
       </c>
@@ -1023,14 +1057,17 @@
         <f t="shared" si="1"/>
         <v>0.92592592592592593</v>
       </c>
-      <c r="P13" s="27">
+      <c r="P13" s="28">
         <v>0.64236111111111105</v>
       </c>
-      <c r="Q13" s="28">
+      <c r="Q13" s="29">
         <v>0.64340277777777777</v>
       </c>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R13" s="31" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" s="10">
         <v>2</v>
       </c>
@@ -1069,20 +1106,23 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="P14" s="27">
+      <c r="P14" s="28">
         <v>0.64374999999999993</v>
       </c>
-      <c r="Q14" s="28">
+      <c r="Q14" s="29">
         <v>0.64502314814814821</v>
       </c>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R14" s="31" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" s="22" t="s">
         <v>26</v>
       </c>
       <c r="M15" s="24"/>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" s="20">
         <v>4</v>
       </c>
@@ -1121,14 +1161,17 @@
         <f t="shared" si="1"/>
         <v>0.90476190476190477</v>
       </c>
-      <c r="P16" s="27">
+      <c r="P16" s="28">
         <v>0.72152777777777777</v>
       </c>
-      <c r="Q16" s="28">
+      <c r="Q16" s="29">
         <v>0.72313657407407417</v>
       </c>
-    </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R16">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17" s="6">
         <v>4</v>
       </c>
@@ -1167,14 +1210,17 @@
         <f t="shared" si="1"/>
         <v>1.0384615384615385</v>
       </c>
-      <c r="P17" s="27">
+      <c r="P17" s="28">
         <v>0.72361111111111109</v>
       </c>
-      <c r="Q17" s="28">
+      <c r="Q17" s="29">
         <v>0.72545138888888883</v>
       </c>
-    </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R17">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A18" s="6">
         <v>4</v>
       </c>
@@ -1213,14 +1259,17 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="P18" s="27">
+      <c r="P18" s="28">
         <v>0.72638888888888886</v>
       </c>
-      <c r="Q18" s="28">
+      <c r="Q18" s="29">
         <v>0.72768518518518521</v>
       </c>
-    </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R18">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19" s="10">
         <v>4</v>
       </c>
@@ -1259,29 +1308,442 @@
         <f t="shared" si="1"/>
         <v>0.91666666666666663</v>
       </c>
-      <c r="P19" s="27">
+      <c r="P19" s="28">
         <v>0.7284722222222223</v>
       </c>
-      <c r="Q19" s="28">
+      <c r="Q19" s="29">
         <v>0.72949074074074083</v>
       </c>
-    </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R19" s="31" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
       <c r="M21" s="19">
         <f>AVERAGE(M6:M19)</f>
         <v>0.93212728629395292</v>
       </c>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
       <c r="M22" s="24">
         <f>_xlfn.STDEV.P(M6:M20)</f>
         <v>8.0677889952617779E-2</v>
       </c>
     </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A26" s="2"/>
+      <c r="B26" s="3"/>
+      <c r="C26" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="D26" s="30"/>
+      <c r="E26" s="30"/>
+      <c r="F26" s="27"/>
+      <c r="G26" s="30" t="s">
+        <v>7</v>
+      </c>
+      <c r="H26" s="30"/>
+      <c r="I26" s="30"/>
+      <c r="J26" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="K26" s="5"/>
+      <c r="L26" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="M26" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A27" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B27" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="C27" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="D27" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="E27" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="F27" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="G27" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="H27" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="I27" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="J27" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="K27" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="L27" s="14"/>
+      <c r="P27" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q27" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A28" s="6">
+        <v>3</v>
+      </c>
+      <c r="B28" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C28" s="7">
+        <v>15</v>
+      </c>
+      <c r="D28" s="7">
+        <v>0</v>
+      </c>
+      <c r="E28" s="15"/>
+      <c r="F28" s="15">
+        <v>2</v>
+      </c>
+      <c r="G28" s="15"/>
+      <c r="H28" s="7"/>
+      <c r="I28" s="7"/>
+      <c r="J28" s="7">
+        <v>28</v>
+      </c>
+      <c r="K28" s="8"/>
+      <c r="L28" s="8"/>
+      <c r="M28" s="19">
+        <f>(C28-D28)/J28</f>
+        <v>0.5357142857142857</v>
+      </c>
+      <c r="P28" s="28">
+        <v>0.60972222222222217</v>
+      </c>
+      <c r="Q28" s="29">
+        <v>0.61226851851851849</v>
+      </c>
+      <c r="R28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A29" s="6">
+        <v>3</v>
+      </c>
+      <c r="B29" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C29" s="7">
+        <v>15</v>
+      </c>
+      <c r="D29" s="7">
+        <v>1</v>
+      </c>
+      <c r="E29" s="15"/>
+      <c r="F29" s="15">
+        <v>2</v>
+      </c>
+      <c r="G29" s="15"/>
+      <c r="H29" s="15"/>
+      <c r="I29" s="15"/>
+      <c r="J29" s="7">
+        <v>27</v>
+      </c>
+      <c r="K29" s="8"/>
+      <c r="L29" s="8"/>
+      <c r="M29" s="19">
+        <f t="shared" ref="M29:M31" si="2">(C29-D29)/J29</f>
+        <v>0.51851851851851849</v>
+      </c>
+      <c r="P29" s="28">
+        <v>0.61458333333333337</v>
+      </c>
+      <c r="Q29" s="29">
+        <v>0.61684027777777783</v>
+      </c>
+      <c r="R29">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A30" s="6">
+        <v>3</v>
+      </c>
+      <c r="B30" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="C30" s="7">
+        <v>12</v>
+      </c>
+      <c r="D30" s="7">
+        <v>1</v>
+      </c>
+      <c r="E30" s="7"/>
+      <c r="F30" s="15"/>
+      <c r="G30" s="7"/>
+      <c r="H30" s="7"/>
+      <c r="I30" s="7"/>
+      <c r="J30" s="7">
+        <v>33</v>
+      </c>
+      <c r="K30" s="8"/>
+      <c r="L30" s="8"/>
+      <c r="M30" s="19">
+        <f t="shared" si="2"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="P30" s="28">
+        <v>0.61805555555555558</v>
+      </c>
+      <c r="Q30" s="29">
+        <v>0.61962962962962964</v>
+      </c>
+      <c r="R30">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A31" s="10">
+        <v>3</v>
+      </c>
+      <c r="B31" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="C31" s="11"/>
+      <c r="D31" s="11"/>
+      <c r="E31" s="11"/>
+      <c r="F31" s="17"/>
+      <c r="G31" s="11"/>
+      <c r="H31" s="11"/>
+      <c r="I31" s="17"/>
+      <c r="J31" s="11">
+        <v>32</v>
+      </c>
+      <c r="K31" s="12"/>
+      <c r="L31" s="12"/>
+      <c r="M31" s="19">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="P31" s="28">
+        <v>0.62013888888888891</v>
+      </c>
+      <c r="Q31" s="29">
+        <v>0.62229166666666669</v>
+      </c>
+      <c r="R31">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A32" s="18" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A33" s="20">
+        <v>2</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C33" s="21"/>
+      <c r="D33" s="3"/>
+      <c r="E33" s="3"/>
+      <c r="F33" s="3"/>
+      <c r="G33" s="3"/>
+      <c r="H33" s="3"/>
+      <c r="I33" s="3"/>
+      <c r="J33" s="3">
+        <v>24</v>
+      </c>
+      <c r="K33" s="3"/>
+      <c r="L33" s="5"/>
+      <c r="M33" s="24">
+        <f>(C33-D33)/J33</f>
+        <v>0</v>
+      </c>
+      <c r="P33" s="28">
+        <v>0.63402777777777775</v>
+      </c>
+      <c r="Q33" s="29">
+        <v>0.63670138888888894</v>
+      </c>
+      <c r="R33">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A34" s="6">
+        <v>2</v>
+      </c>
+      <c r="B34" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C34" s="23"/>
+      <c r="D34" s="15"/>
+      <c r="E34" s="15"/>
+      <c r="F34" s="15"/>
+      <c r="G34" s="15"/>
+      <c r="H34" s="15"/>
+      <c r="I34" s="15"/>
+      <c r="J34" s="15">
+        <v>27</v>
+      </c>
+      <c r="K34" s="15"/>
+      <c r="L34" s="8"/>
+      <c r="M34" s="24">
+        <f>(C34-D34)/J34</f>
+        <v>0</v>
+      </c>
+      <c r="P34" s="28">
+        <v>0.6381944444444444</v>
+      </c>
+      <c r="Q34" s="29">
+        <v>0.64165509259259257</v>
+      </c>
+      <c r="R34">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A35" s="22" t="s">
+        <v>26</v>
+      </c>
+      <c r="M35" s="24"/>
+    </row>
+    <row r="36" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A36" s="20">
+        <v>4</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C36" s="26"/>
+      <c r="D36" s="3"/>
+      <c r="E36" s="3"/>
+      <c r="F36" s="3"/>
+      <c r="G36" s="3"/>
+      <c r="H36" s="3"/>
+      <c r="I36" s="3"/>
+      <c r="J36" s="3">
+        <v>21</v>
+      </c>
+      <c r="K36" s="3"/>
+      <c r="L36" s="5"/>
+      <c r="M36" s="24">
+        <f>(C36-D36)/J33</f>
+        <v>0</v>
+      </c>
+      <c r="P36" s="28">
+        <v>0.72152777777777777</v>
+      </c>
+      <c r="Q36" s="29">
+        <v>0.72313657407407417</v>
+      </c>
+      <c r="R36">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A37" s="6">
+        <v>4</v>
+      </c>
+      <c r="B37" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C37" s="23"/>
+      <c r="D37" s="15"/>
+      <c r="E37" s="15"/>
+      <c r="F37" s="15"/>
+      <c r="G37" s="15"/>
+      <c r="H37" s="15"/>
+      <c r="I37" s="15"/>
+      <c r="J37" s="15">
+        <v>26</v>
+      </c>
+      <c r="K37" s="15"/>
+      <c r="L37" s="8"/>
+      <c r="M37" s="24">
+        <f>(C37-D37)/J34</f>
+        <v>0</v>
+      </c>
+      <c r="P37" s="28">
+        <v>0.72361111111111109</v>
+      </c>
+      <c r="Q37" s="29">
+        <v>0.72545138888888883</v>
+      </c>
+      <c r="R37">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A38" s="6">
+        <v>4</v>
+      </c>
+      <c r="B38" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C38" s="23"/>
+      <c r="D38" s="15"/>
+      <c r="E38" s="15"/>
+      <c r="F38" s="15"/>
+      <c r="G38" s="15"/>
+      <c r="H38" s="15"/>
+      <c r="I38" s="15"/>
+      <c r="J38" s="15">
+        <v>13</v>
+      </c>
+      <c r="K38" s="15"/>
+      <c r="L38" s="8"/>
+      <c r="M38" s="24">
+        <f t="shared" ref="M36:M38" si="3">(C38-D38)/J38</f>
+        <v>0</v>
+      </c>
+      <c r="P38" s="28">
+        <v>0.72638888888888886</v>
+      </c>
+      <c r="Q38" s="29">
+        <v>0.72768518518518521</v>
+      </c>
+      <c r="R38">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="40" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="M40" s="19">
+        <f>AVERAGE(M28:M38)</f>
+        <v>0.15417401528512639</v>
+      </c>
+    </row>
+    <row r="41" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="M41" s="24">
+        <f>_xlfn.STDEV.P(M28:M39)</f>
+        <v>0.22435976024973628</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="4">
     <mergeCell ref="C4:E4"/>
     <mergeCell ref="G4:I4"/>
+    <mergeCell ref="C26:E26"/>
+    <mergeCell ref="G26:I26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>